<commit_message>
aggiunto creazione foglio excel
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,12 @@
     <t>13-11-21</t>
   </si>
   <si>
+    <t>15-11-21</t>
+  </si>
+  <si>
+    <t>16-11-21</t>
+  </si>
+  <si>
     <t>14:11</t>
   </si>
   <si>
@@ -49,6 +55,45 @@
     <t>19:16</t>
   </si>
   <si>
+    <t>23:42</t>
+  </si>
+  <si>
+    <t>16:57</t>
+  </si>
+  <si>
+    <t>17:04</t>
+  </si>
+  <si>
+    <t>17:13</t>
+  </si>
+  <si>
+    <t>17:15</t>
+  </si>
+  <si>
+    <t>17:58</t>
+  </si>
+  <si>
+    <t>19:10</t>
+  </si>
+  <si>
+    <t>11:16</t>
+  </si>
+  <si>
+    <t>11:23</t>
+  </si>
+  <si>
+    <t>11:27</t>
+  </si>
+  <si>
+    <t>11:28</t>
+  </si>
+  <si>
+    <t>11:29</t>
+  </si>
+  <si>
+    <t>11:35</t>
+  </si>
+  <si>
     <t>jhbhb</t>
   </si>
   <si>
@@ -64,6 +109,45 @@
     <t>yvy</t>
   </si>
   <si>
+    <t>dsiofsdif</t>
+  </si>
+  <si>
+    <t>uggu</t>
+  </si>
+  <si>
+    <t>derf</t>
+  </si>
+  <si>
+    <t>edewd</t>
+  </si>
+  <si>
+    <t>sdasssdsadsdsadasdsad</t>
+  </si>
+  <si>
+    <t>sdd</t>
+  </si>
+  <si>
+    <t>sdsad</t>
+  </si>
+  <si>
+    <t>dasdsad</t>
+  </si>
+  <si>
+    <t>xczxc</t>
+  </si>
+  <si>
+    <t>sadasd</t>
+  </si>
+  <si>
+    <t>dsdsad</t>
+  </si>
+  <si>
+    <t>CNTFBA75P24H501P</t>
+  </si>
+  <si>
+    <t>dss</t>
+  </si>
+  <si>
     <t>dxd</t>
   </si>
   <si>
@@ -77,6 +161,39 @@
   </si>
   <si>
     <t>vyyvy</t>
+  </si>
+  <si>
+    <t>iniunin</t>
+  </si>
+  <si>
+    <t>guybub</t>
+  </si>
+  <si>
+    <t>crct</t>
+  </si>
+  <si>
+    <t>ewede</t>
+  </si>
+  <si>
+    <t>sadsadsadsadsadasdsadsad</t>
+  </si>
+  <si>
+    <t>dsads</t>
+  </si>
+  <si>
+    <t>sdsads</t>
+  </si>
+  <si>
+    <t>sadsadsad</t>
+  </si>
+  <si>
+    <t>czxcxzc</t>
+  </si>
+  <si>
+    <t>sdasd</t>
+  </si>
+  <si>
+    <t>sadsadas</t>
   </si>
 </sst>
 </file>
@@ -434,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,13 +585,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -488,13 +605,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -508,13 +625,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -528,13 +645,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -548,16 +665,376 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18">
+        <v>99914130540219</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>1.603008416904999E+26</v>
+      </c>
+      <c r="E19">
+        <v>99914130540219</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20">
+        <v>99914130540219</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21">
+        <v>1603008416904</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>1603008416904</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>99914130540219</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>